<commit_message>
added dateSerial funciton to convert jsDate to xlDate
</commit_message>
<xml_diff>
--- a/test/reports/events-list/events-list-template.xlsx
+++ b/test/reports/events-list/events-list-template.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="events" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">events!$A$1:$W$2</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,73 +25,73 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
-    <t xml:space="preserve">internal-build-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">external-build-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event-from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">event-to</t>
-  </si>
-  <si>
-    <t xml:space="preserve">external-dismantling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">internal-dismantling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matchcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">technician</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd-manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd-tpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd-technician</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd-plm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd-security</t>
+    <t xml:space="preserve">Interner Aufbau ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Externer Aufbau ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VA ab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VA bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Externer Abbau bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inerner Abbau bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matchcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicherheit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technik2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicherheit2</t>
   </si>
   <si>
     <t xml:space="preserve">#! FOR_EACH item data</t>
@@ -173,8 +176,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -250,7 +254,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,6 +264,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,6 +283,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -283,7 +295,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -390,22 +402,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -604,6 +616,7 @@
       <c r="K9" s="0"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -611,5 +624,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>